<commit_message>
Doplneni resolve pro Future pri odeslani zpravy
</commit_message>
<xml_diff>
--- a/prez/KafkaCLICheatsheet.xlsx
+++ b/prez/KafkaCLICheatsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lisak/Projects/test/KafkaVKostce/prez/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE32DAF-82A0-BB45-9418-31986F10E184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CAC7F07-4B74-184E-BADF-F40735A49B10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="5400" windowWidth="32820" windowHeight="19500" xr2:uid="{43CCA812-24B0-8D47-A175-C597BF9E8CF7}"/>
+    <workbookView xWindow="17240" yWindow="8280" windowWidth="32820" windowHeight="19500" xr2:uid="{43CCA812-24B0-8D47-A175-C597BF9E8CF7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,10 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
-  <si>
-    <t>kafka-topics --bootstrap-server $BOOT --create --topic moon-landings --partitions 3</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Manuální založení topicu s daným počtem partitions a defaultním replikačním faktorem</t>
   </si>
@@ -46,42 +43,24 @@
     <t>Manuální založení topicu s daným počtem partitions a explicitním replikačním faktorem</t>
   </si>
   <si>
-    <t>kafka-topics --bootstrap-server $BOOT --create --topic moon-landings --partitions 3 --replication-factor 2</t>
-  </si>
-  <si>
-    <t>kafka-topics --bootstrap-server $BOOT --describe --topic moon-landings</t>
-  </si>
-  <si>
     <t>Výpis informací o konkrétním topicu</t>
   </si>
   <si>
-    <t>kafka-console-producer --bootstrap-server $BOOT --topic moon-landings --property parse.key=true --property key.separator=:</t>
-  </si>
-  <si>
     <t>Manuální odeslání zprávy z konzole - co řádek, to zpráva; formát zprávy &lt;klíč&gt;:&lt;hodnota&gt;</t>
   </si>
   <si>
     <t>Příjem zprávy od začátku topicu, včetně informací o partition a offsetu</t>
   </si>
   <si>
-    <t>kafka-console-consumer --bootstrap-server $BOOT --topic moon-landings --from-beginning --property print.key=true --property print.value=true --property print.partition=true --property print.offset=true</t>
-  </si>
-  <si>
     <t>Příjem zprávy od začátku topicu v rámci consumer grupy "g1"</t>
   </si>
   <si>
-    <t>kafka-console-consumer --bootstrap-server $BOOT --topic moon-landings --property print.key=true --property print.value=true --property print.partition=true --property print.offset=true --group g1</t>
-  </si>
-  <si>
     <t>kafka-consumer-groups --bootstrap-server $BOOT --group g1 --describe</t>
   </si>
   <si>
     <t>kafka-consumer-groups --bootstrap-server $BOOT --group g1 --describe --members --verbose</t>
   </si>
   <si>
-    <t>kafka-consumer-groups --bootstrap-server $BOOT --topic moon-landings --describe</t>
-  </si>
-  <si>
     <t>Výpis informací o topicu - partitions, leader, repliky</t>
   </si>
   <si>
@@ -89,6 +68,39 @@
   </si>
   <si>
     <t>Výpis informací o consumer grupě - aktuální offset a lag jednotlivých consumerů</t>
+  </si>
+  <si>
+    <t>Seznam topiců na brokeru</t>
+  </si>
+  <si>
+    <t>kafka-topics --bootstrap-server=$BOOT --list</t>
+  </si>
+  <si>
+    <t>kafka-topics --bootstrap-server $BOOT --create --topic lunar-landings --partitions 3</t>
+  </si>
+  <si>
+    <t>kafka-topics --bootstrap-server $BOOT --create --topic lunar-landings --partitions 3 --replication-factor 2</t>
+  </si>
+  <si>
+    <t>kafka-topics --bootstrap-server $BOOT --describe --topic lunar-landings</t>
+  </si>
+  <si>
+    <t>kafka-console-producer --bootstrap-server $BOOT --topic lunar-landings --property parse.key=true --property key.separator=:</t>
+  </si>
+  <si>
+    <t>kafka-console-consumer --bootstrap-server $BOOT --topic lunar-landings --from-beginning --property print.key=true --property print.value=true --property print.partition=true --property print.offset=true</t>
+  </si>
+  <si>
+    <t>kafka-console-consumer --bootstrap-server $BOOT --topic lunar-landings --property print.key=true --property print.value=true --property print.partition=true --property print.offset=true --group g1</t>
+  </si>
+  <si>
+    <t>kafka-consumer-groups --bootstrap-server $BOOT --topic lunar-landings --describe</t>
+  </si>
+  <si>
+    <t>Seznam všech existujících consumer groups</t>
+  </si>
+  <si>
+    <t>kafka-consumer-groups --bootstrap-server $BOOT --list</t>
   </si>
 </sst>
 </file>
@@ -449,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3A71F7C-E787-1E4A-AEC5-0B64A8847AB4}">
-  <dimension ref="A2:B10"/>
+  <dimension ref="A2:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -464,74 +476,90 @@
   <sheetData>
     <row r="2" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>